<commit_message>
Incorporating major and minor genotypes from Grubaugh lab
</commit_message>
<xml_diff>
--- a/tabular/denv_reference_data.xlsx
+++ b/tabular/denv_reference_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/Dengue-GLUE/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEAA6FC-36B8-2440-8E9B-2E74805386FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45105B62-F9D2-4D4B-A79D-BDE175C16B23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="500" windowWidth="27560" windowHeight="17040" xr2:uid="{3983FCA1-51FF-C04D-9A81-E3489DB1D9F2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="550">
   <si>
     <t>1IV_NC_001477</t>
   </si>
@@ -1680,9 +1680,6 @@
   </si>
   <si>
     <t>rDEN4</t>
-  </si>
-  <si>
-    <t>1VI</t>
   </si>
   <si>
     <t>serotype</t>
@@ -2071,8 +2068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5813ACA-0E75-F841-9157-B1D7C72560FD}">
   <dimension ref="A1:L147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E106" sqref="A1:L147"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D33" sqref="A1:L147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2095,7 +2092,7 @@
         <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>536</v>
@@ -3224,7 +3221,7 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>549</v>
+        <v>61</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>352</v>
@@ -3253,7 +3250,7 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>549</v>
+        <v>61</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>372</v>

</xml_diff>